<commit_message>
implementando 2 canetas otimizado
</commit_message>
<xml_diff>
--- a/INFESTOS/Ficha técnica.xlsx
+++ b/INFESTOS/Ficha técnica.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="36" uniqueCount="33">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="40" uniqueCount="37">
   <si>
     <t>Laser Cut Infestos</t>
   </si>
@@ -115,6 +115,18 @@
   </si>
   <si>
     <t>89cm/36un</t>
+  </si>
+  <si>
+    <t>JA3 P</t>
+  </si>
+  <si>
+    <t>JA3 M</t>
+  </si>
+  <si>
+    <t>JA3 G</t>
+  </si>
+  <si>
+    <t>JA3 GG</t>
   </si>
 </sst>
 </file>
@@ -427,36 +439,81 @@
   <cellXfs count="33">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="17" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="6" xfId="0" quotePrefix="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="20" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="18" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="19" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -473,51 +530,6 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="17" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="17" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="18" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="19" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="6" xfId="0" quotePrefix="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="20" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
@@ -817,7 +829,7 @@
   <dimension ref="A1:J50"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E14" sqref="E14"/>
+      <selection activeCell="A19" sqref="A19:C19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -826,520 +838,528 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:10" ht="20.100000000000001" customHeight="1">
-      <c r="A1" s="3" t="s">
+      <c r="A1" s="17" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="4"/>
-      <c r="C1" s="4"/>
-      <c r="D1" s="4"/>
-      <c r="E1" s="4"/>
-      <c r="F1" s="4"/>
-      <c r="G1" s="4"/>
-      <c r="H1" s="4"/>
-      <c r="I1" s="5"/>
-      <c r="J1" s="7"/>
+      <c r="B1" s="18"/>
+      <c r="C1" s="18"/>
+      <c r="D1" s="18"/>
+      <c r="E1" s="18"/>
+      <c r="F1" s="18"/>
+      <c r="G1" s="18"/>
+      <c r="H1" s="18"/>
+      <c r="I1" s="19"/>
+      <c r="J1" s="3"/>
     </row>
     <row r="2" spans="1:10" ht="20.100000000000001" customHeight="1" thickBot="1">
-      <c r="A2" s="8"/>
-      <c r="B2" s="2"/>
-      <c r="C2" s="2"/>
-      <c r="D2" s="2"/>
-      <c r="E2" s="2"/>
-      <c r="F2" s="2"/>
-      <c r="G2" s="2"/>
-      <c r="H2" s="2"/>
-      <c r="I2" s="9"/>
-      <c r="J2" s="7"/>
+      <c r="A2" s="20"/>
+      <c r="B2" s="21"/>
+      <c r="C2" s="21"/>
+      <c r="D2" s="21"/>
+      <c r="E2" s="21"/>
+      <c r="F2" s="21"/>
+      <c r="G2" s="21"/>
+      <c r="H2" s="21"/>
+      <c r="I2" s="22"/>
+      <c r="J2" s="3"/>
     </row>
     <row r="3" spans="1:10" ht="20.100000000000001" customHeight="1" thickBot="1">
-      <c r="A3" s="16" t="s">
+      <c r="A3" s="31" t="s">
         <v>3</v>
       </c>
-      <c r="B3" s="17"/>
-      <c r="C3" s="17"/>
-      <c r="D3" s="18" t="s">
+      <c r="B3" s="32"/>
+      <c r="C3" s="32"/>
+      <c r="D3" s="4" t="s">
         <v>26</v>
       </c>
-      <c r="E3" s="18" t="s">
+      <c r="E3" s="4" t="s">
         <v>1</v>
       </c>
-      <c r="F3" s="18" t="s">
+      <c r="F3" s="4" t="s">
         <v>2</v>
       </c>
-      <c r="G3" s="18" t="s">
+      <c r="G3" s="4" t="s">
         <v>27</v>
       </c>
-      <c r="H3" s="19" t="s">
+      <c r="H3" s="15" t="s">
         <v>13</v>
       </c>
-      <c r="I3" s="20"/>
-      <c r="J3" s="6"/>
+      <c r="I3" s="16"/>
+      <c r="J3" s="2"/>
     </row>
     <row r="4" spans="1:10" ht="20.100000000000001" customHeight="1">
-      <c r="A4" s="14" t="s">
+      <c r="A4" s="29" t="s">
         <v>4</v>
       </c>
-      <c r="B4" s="15"/>
-      <c r="C4" s="15"/>
-      <c r="D4" s="21"/>
-      <c r="E4" s="21" t="s">
+      <c r="B4" s="30"/>
+      <c r="C4" s="30"/>
+      <c r="D4" s="5"/>
+      <c r="E4" s="5" t="s">
         <v>16</v>
       </c>
-      <c r="F4" s="21" t="s">
+      <c r="F4" s="5" t="s">
         <v>17</v>
       </c>
-      <c r="G4" s="21"/>
-      <c r="H4" s="22"/>
-      <c r="I4" s="23"/>
-      <c r="J4" s="6"/>
+      <c r="G4" s="5"/>
+      <c r="H4" s="23"/>
+      <c r="I4" s="24"/>
+      <c r="J4" s="2"/>
     </row>
     <row r="5" spans="1:10" ht="20.100000000000001" customHeight="1">
-      <c r="A5" s="11" t="s">
+      <c r="A5" s="25" t="s">
         <v>5</v>
       </c>
-      <c r="B5" s="10"/>
-      <c r="C5" s="10"/>
-      <c r="D5" s="24"/>
-      <c r="E5" s="24" t="s">
+      <c r="B5" s="26"/>
+      <c r="C5" s="26"/>
+      <c r="D5" s="6"/>
+      <c r="E5" s="6" t="s">
         <v>18</v>
       </c>
-      <c r="F5" s="25" t="s">
+      <c r="F5" s="7" t="s">
         <v>19</v>
       </c>
-      <c r="G5" s="25"/>
-      <c r="H5" s="26"/>
-      <c r="I5" s="27"/>
-      <c r="J5" s="6"/>
+      <c r="G5" s="7"/>
+      <c r="H5" s="11"/>
+      <c r="I5" s="12"/>
+      <c r="J5" s="2"/>
     </row>
     <row r="6" spans="1:10" ht="20.100000000000001" customHeight="1">
-      <c r="A6" s="11" t="s">
+      <c r="A6" s="25" t="s">
         <v>6</v>
       </c>
-      <c r="B6" s="10"/>
-      <c r="C6" s="10"/>
-      <c r="D6" s="24"/>
-      <c r="E6" s="24" t="s">
+      <c r="B6" s="26"/>
+      <c r="C6" s="26"/>
+      <c r="D6" s="6"/>
+      <c r="E6" s="6" t="s">
         <v>21</v>
       </c>
-      <c r="F6" s="24"/>
-      <c r="G6" s="24"/>
-      <c r="H6" s="26" t="s">
+      <c r="F6" s="6"/>
+      <c r="G6" s="6"/>
+      <c r="H6" s="11" t="s">
         <v>20</v>
       </c>
-      <c r="I6" s="27"/>
-      <c r="J6" s="6"/>
+      <c r="I6" s="12"/>
+      <c r="J6" s="2"/>
     </row>
     <row r="7" spans="1:10" ht="20.100000000000001" customHeight="1">
-      <c r="A7" s="11" t="s">
+      <c r="A7" s="25" t="s">
         <v>8</v>
       </c>
-      <c r="B7" s="10"/>
-      <c r="C7" s="10"/>
-      <c r="D7" s="24"/>
-      <c r="E7" s="24" t="s">
+      <c r="B7" s="26"/>
+      <c r="C7" s="26"/>
+      <c r="D7" s="6"/>
+      <c r="E7" s="6" t="s">
         <v>22</v>
       </c>
-      <c r="F7" s="24" t="s">
+      <c r="F7" s="6" t="s">
         <v>22</v>
       </c>
-      <c r="G7" s="24"/>
-      <c r="H7" s="26"/>
-      <c r="I7" s="27"/>
-      <c r="J7" s="6"/>
+      <c r="G7" s="6"/>
+      <c r="H7" s="11"/>
+      <c r="I7" s="12"/>
+      <c r="J7" s="2"/>
     </row>
     <row r="8" spans="1:10" ht="20.100000000000001" customHeight="1">
-      <c r="A8" s="11" t="s">
+      <c r="A8" s="25" t="s">
         <v>9</v>
       </c>
-      <c r="B8" s="10"/>
-      <c r="C8" s="10"/>
-      <c r="D8" s="24"/>
-      <c r="E8" s="24" t="s">
+      <c r="B8" s="26"/>
+      <c r="C8" s="26"/>
+      <c r="D8" s="6"/>
+      <c r="E8" s="6" t="s">
         <v>23</v>
       </c>
-      <c r="F8" s="24" t="s">
+      <c r="F8" s="6" t="s">
         <v>23</v>
       </c>
-      <c r="G8" s="24"/>
-      <c r="H8" s="26"/>
-      <c r="I8" s="27"/>
-      <c r="J8" s="6"/>
+      <c r="G8" s="6"/>
+      <c r="H8" s="11"/>
+      <c r="I8" s="12"/>
+      <c r="J8" s="2"/>
     </row>
     <row r="9" spans="1:10" ht="20.100000000000001" customHeight="1">
-      <c r="A9" s="11" t="s">
+      <c r="A9" s="25" t="s">
         <v>10</v>
       </c>
-      <c r="B9" s="10"/>
-      <c r="C9" s="10"/>
-      <c r="D9" s="24"/>
-      <c r="E9" s="24"/>
-      <c r="F9" s="24"/>
-      <c r="G9" s="24"/>
-      <c r="H9" s="26"/>
-      <c r="I9" s="27"/>
-      <c r="J9" s="6"/>
+      <c r="B9" s="26"/>
+      <c r="C9" s="26"/>
+      <c r="D9" s="6"/>
+      <c r="E9" s="6"/>
+      <c r="F9" s="6"/>
+      <c r="G9" s="6"/>
+      <c r="H9" s="11"/>
+      <c r="I9" s="12"/>
+      <c r="J9" s="2"/>
     </row>
     <row r="10" spans="1:10" ht="20.100000000000001" customHeight="1">
-      <c r="A10" s="11" t="s">
+      <c r="A10" s="25" t="s">
         <v>7</v>
       </c>
-      <c r="B10" s="10"/>
-      <c r="C10" s="10"/>
-      <c r="D10" s="24"/>
-      <c r="E10" s="24" t="s">
+      <c r="B10" s="26"/>
+      <c r="C10" s="26"/>
+      <c r="D10" s="6"/>
+      <c r="E10" s="6" t="s">
         <v>24</v>
       </c>
-      <c r="F10" s="24" t="s">
+      <c r="F10" s="6" t="s">
         <v>24</v>
       </c>
-      <c r="G10" s="24"/>
-      <c r="H10" s="26"/>
-      <c r="I10" s="27"/>
-      <c r="J10" s="6"/>
+      <c r="G10" s="6"/>
+      <c r="H10" s="11"/>
+      <c r="I10" s="12"/>
+      <c r="J10" s="2"/>
     </row>
     <row r="11" spans="1:10" ht="20.100000000000001" customHeight="1">
-      <c r="A11" s="11" t="s">
+      <c r="A11" s="25" t="s">
         <v>11</v>
       </c>
-      <c r="B11" s="10"/>
-      <c r="C11" s="10"/>
-      <c r="D11" s="24"/>
-      <c r="E11" s="24" t="s">
+      <c r="B11" s="26"/>
+      <c r="C11" s="26"/>
+      <c r="D11" s="6"/>
+      <c r="E11" s="6" t="s">
         <v>25</v>
       </c>
-      <c r="F11" s="24"/>
-      <c r="G11" s="24"/>
-      <c r="H11" s="26"/>
-      <c r="I11" s="27"/>
-      <c r="J11" s="6"/>
+      <c r="F11" s="6"/>
+      <c r="G11" s="6"/>
+      <c r="H11" s="11"/>
+      <c r="I11" s="12"/>
+      <c r="J11" s="2"/>
     </row>
     <row r="12" spans="1:10" ht="20.100000000000001" customHeight="1">
-      <c r="A12" s="11" t="s">
+      <c r="A12" s="25" t="s">
         <v>12</v>
       </c>
-      <c r="B12" s="10"/>
-      <c r="C12" s="10"/>
-      <c r="D12" s="24"/>
-      <c r="E12" s="31" t="s">
+      <c r="B12" s="26"/>
+      <c r="C12" s="26"/>
+      <c r="D12" s="6"/>
+      <c r="E12" s="9" t="s">
         <v>28</v>
       </c>
-      <c r="F12" s="24"/>
-      <c r="G12" s="24"/>
-      <c r="H12" s="26"/>
-      <c r="I12" s="27"/>
-      <c r="J12" s="6"/>
+      <c r="F12" s="6"/>
+      <c r="G12" s="6"/>
+      <c r="H12" s="11"/>
+      <c r="I12" s="12"/>
+      <c r="J12" s="2"/>
     </row>
     <row r="13" spans="1:10" ht="20.100000000000001" customHeight="1">
-      <c r="A13" s="11" t="s">
+      <c r="A13" s="25" t="s">
         <v>14</v>
       </c>
-      <c r="B13" s="10"/>
-      <c r="C13" s="10"/>
-      <c r="D13" s="24"/>
-      <c r="E13" s="31" t="s">
+      <c r="B13" s="26"/>
+      <c r="C13" s="26"/>
+      <c r="D13" s="6"/>
+      <c r="E13" s="9" t="s">
         <v>29</v>
       </c>
-      <c r="F13" s="24"/>
-      <c r="G13" s="24" t="s">
+      <c r="F13" s="6"/>
+      <c r="G13" s="6" t="s">
         <v>31</v>
       </c>
-      <c r="H13" s="26" t="s">
+      <c r="H13" s="11" t="s">
         <v>30</v>
       </c>
-      <c r="I13" s="27"/>
-      <c r="J13" s="6"/>
+      <c r="I13" s="12"/>
+      <c r="J13" s="2"/>
     </row>
     <row r="14" spans="1:10" ht="20.100000000000001" customHeight="1">
-      <c r="A14" s="11" t="s">
+      <c r="A14" s="25" t="s">
         <v>15</v>
       </c>
-      <c r="B14" s="10"/>
-      <c r="C14" s="10"/>
-      <c r="D14" s="24"/>
-      <c r="E14" s="31" t="s">
+      <c r="B14" s="26"/>
+      <c r="C14" s="26"/>
+      <c r="D14" s="6"/>
+      <c r="E14" s="9" t="s">
         <v>32</v>
       </c>
-      <c r="F14" s="24"/>
-      <c r="G14" s="24"/>
-      <c r="H14" s="26"/>
-      <c r="I14" s="27"/>
-      <c r="J14" s="6"/>
+      <c r="F14" s="6"/>
+      <c r="G14" s="6"/>
+      <c r="H14" s="11"/>
+      <c r="I14" s="12"/>
+      <c r="J14" s="2"/>
     </row>
     <row r="15" spans="1:10" ht="20.100000000000001" customHeight="1">
-      <c r="A15" s="11"/>
-      <c r="B15" s="10"/>
-      <c r="C15" s="10"/>
-      <c r="D15" s="24"/>
-      <c r="E15" s="31"/>
-      <c r="F15" s="24"/>
-      <c r="G15" s="24"/>
-      <c r="H15" s="26"/>
-      <c r="I15" s="27"/>
-      <c r="J15" s="6"/>
+      <c r="A15" s="25" t="s">
+        <v>33</v>
+      </c>
+      <c r="B15" s="26"/>
+      <c r="C15" s="26"/>
+      <c r="D15" s="6"/>
+      <c r="E15" s="9"/>
+      <c r="F15" s="6"/>
+      <c r="G15" s="6"/>
+      <c r="H15" s="11"/>
+      <c r="I15" s="12"/>
+      <c r="J15" s="2"/>
     </row>
     <row r="16" spans="1:10" ht="20.100000000000001" customHeight="1">
-      <c r="A16" s="11"/>
-      <c r="B16" s="10"/>
-      <c r="C16" s="10"/>
-      <c r="D16" s="24"/>
-      <c r="E16" s="31"/>
-      <c r="F16" s="24"/>
-      <c r="G16" s="24"/>
-      <c r="H16" s="26"/>
-      <c r="I16" s="27"/>
-      <c r="J16" s="6"/>
+      <c r="A16" s="25" t="s">
+        <v>34</v>
+      </c>
+      <c r="B16" s="26"/>
+      <c r="C16" s="26"/>
+      <c r="D16" s="6"/>
+      <c r="E16" s="9"/>
+      <c r="F16" s="6"/>
+      <c r="G16" s="6"/>
+      <c r="H16" s="11"/>
+      <c r="I16" s="12"/>
+      <c r="J16" s="2"/>
     </row>
     <row r="17" spans="1:10" ht="20.100000000000001" customHeight="1">
-      <c r="A17" s="11"/>
-      <c r="B17" s="10"/>
-      <c r="C17" s="10"/>
-      <c r="D17" s="24"/>
-      <c r="E17" s="31"/>
-      <c r="F17" s="24"/>
-      <c r="G17" s="24"/>
-      <c r="H17" s="26"/>
-      <c r="I17" s="27"/>
-      <c r="J17" s="6"/>
+      <c r="A17" s="25" t="s">
+        <v>35</v>
+      </c>
+      <c r="B17" s="26"/>
+      <c r="C17" s="26"/>
+      <c r="D17" s="6"/>
+      <c r="E17" s="9"/>
+      <c r="F17" s="6"/>
+      <c r="G17" s="6"/>
+      <c r="H17" s="11"/>
+      <c r="I17" s="12"/>
+      <c r="J17" s="2"/>
     </row>
     <row r="18" spans="1:10" ht="20.100000000000001" customHeight="1">
-      <c r="A18" s="11"/>
-      <c r="B18" s="10"/>
-      <c r="C18" s="10"/>
-      <c r="D18" s="24"/>
-      <c r="E18" s="31"/>
-      <c r="F18" s="24"/>
-      <c r="G18" s="24"/>
-      <c r="H18" s="26"/>
-      <c r="I18" s="27"/>
-      <c r="J18" s="6"/>
+      <c r="A18" s="25" t="s">
+        <v>36</v>
+      </c>
+      <c r="B18" s="26"/>
+      <c r="C18" s="26"/>
+      <c r="D18" s="6"/>
+      <c r="E18" s="9"/>
+      <c r="F18" s="6"/>
+      <c r="G18" s="6"/>
+      <c r="H18" s="11"/>
+      <c r="I18" s="12"/>
+      <c r="J18" s="2"/>
     </row>
     <row r="19" spans="1:10" ht="20.100000000000001" customHeight="1">
-      <c r="A19" s="11"/>
-      <c r="B19" s="10"/>
-      <c r="C19" s="10"/>
-      <c r="D19" s="24"/>
-      <c r="E19" s="31"/>
-      <c r="F19" s="24"/>
-      <c r="G19" s="24"/>
-      <c r="H19" s="26"/>
-      <c r="I19" s="27"/>
-      <c r="J19" s="6"/>
+      <c r="A19" s="25"/>
+      <c r="B19" s="26"/>
+      <c r="C19" s="26"/>
+      <c r="D19" s="6"/>
+      <c r="E19" s="9"/>
+      <c r="F19" s="6"/>
+      <c r="G19" s="6"/>
+      <c r="H19" s="11"/>
+      <c r="I19" s="12"/>
+      <c r="J19" s="2"/>
     </row>
     <row r="20" spans="1:10" ht="20.100000000000001" customHeight="1">
-      <c r="A20" s="11"/>
-      <c r="B20" s="10"/>
-      <c r="C20" s="10"/>
-      <c r="D20" s="24"/>
-      <c r="E20" s="31"/>
-      <c r="F20" s="24"/>
-      <c r="G20" s="24"/>
-      <c r="H20" s="26"/>
-      <c r="I20" s="27"/>
-      <c r="J20" s="6"/>
+      <c r="A20" s="25"/>
+      <c r="B20" s="26"/>
+      <c r="C20" s="26"/>
+      <c r="D20" s="6"/>
+      <c r="E20" s="9"/>
+      <c r="F20" s="6"/>
+      <c r="G20" s="6"/>
+      <c r="H20" s="11"/>
+      <c r="I20" s="12"/>
+      <c r="J20" s="2"/>
     </row>
     <row r="21" spans="1:10" ht="20.100000000000001" customHeight="1">
-      <c r="A21" s="11"/>
-      <c r="B21" s="10"/>
-      <c r="C21" s="10"/>
-      <c r="D21" s="24"/>
-      <c r="E21" s="31"/>
-      <c r="F21" s="24"/>
-      <c r="G21" s="24"/>
-      <c r="H21" s="26"/>
-      <c r="I21" s="27"/>
-      <c r="J21" s="6"/>
+      <c r="A21" s="25"/>
+      <c r="B21" s="26"/>
+      <c r="C21" s="26"/>
+      <c r="D21" s="6"/>
+      <c r="E21" s="9"/>
+      <c r="F21" s="6"/>
+      <c r="G21" s="6"/>
+      <c r="H21" s="11"/>
+      <c r="I21" s="12"/>
+      <c r="J21" s="2"/>
     </row>
     <row r="22" spans="1:10" ht="20.100000000000001" customHeight="1">
-      <c r="A22" s="11"/>
-      <c r="B22" s="10"/>
-      <c r="C22" s="10"/>
-      <c r="D22" s="24"/>
-      <c r="E22" s="31"/>
-      <c r="F22" s="24"/>
-      <c r="G22" s="24"/>
-      <c r="H22" s="26"/>
-      <c r="I22" s="27"/>
-      <c r="J22" s="6"/>
+      <c r="A22" s="25"/>
+      <c r="B22" s="26"/>
+      <c r="C22" s="26"/>
+      <c r="D22" s="6"/>
+      <c r="E22" s="9"/>
+      <c r="F22" s="6"/>
+      <c r="G22" s="6"/>
+      <c r="H22" s="11"/>
+      <c r="I22" s="12"/>
+      <c r="J22" s="2"/>
     </row>
     <row r="23" spans="1:10" ht="20.100000000000001" customHeight="1">
-      <c r="A23" s="11"/>
-      <c r="B23" s="10"/>
-      <c r="C23" s="10"/>
-      <c r="D23" s="24"/>
-      <c r="E23" s="31"/>
-      <c r="F23" s="24"/>
-      <c r="G23" s="24"/>
-      <c r="H23" s="26"/>
-      <c r="I23" s="27"/>
-      <c r="J23" s="6"/>
+      <c r="A23" s="25"/>
+      <c r="B23" s="26"/>
+      <c r="C23" s="26"/>
+      <c r="D23" s="6"/>
+      <c r="E23" s="9"/>
+      <c r="F23" s="6"/>
+      <c r="G23" s="6"/>
+      <c r="H23" s="11"/>
+      <c r="I23" s="12"/>
+      <c r="J23" s="2"/>
     </row>
     <row r="24" spans="1:10" ht="20.100000000000001" customHeight="1">
-      <c r="A24" s="11"/>
-      <c r="B24" s="10"/>
-      <c r="C24" s="10"/>
-      <c r="D24" s="24"/>
-      <c r="E24" s="31"/>
-      <c r="F24" s="24"/>
-      <c r="G24" s="24"/>
-      <c r="H24" s="26"/>
-      <c r="I24" s="27"/>
-      <c r="J24" s="6"/>
+      <c r="A24" s="25"/>
+      <c r="B24" s="26"/>
+      <c r="C24" s="26"/>
+      <c r="D24" s="6"/>
+      <c r="E24" s="9"/>
+      <c r="F24" s="6"/>
+      <c r="G24" s="6"/>
+      <c r="H24" s="11"/>
+      <c r="I24" s="12"/>
+      <c r="J24" s="2"/>
     </row>
     <row r="25" spans="1:10" ht="20.100000000000001" customHeight="1">
-      <c r="A25" s="11"/>
-      <c r="B25" s="10"/>
-      <c r="C25" s="10"/>
-      <c r="D25" s="24"/>
-      <c r="E25" s="31"/>
-      <c r="F25" s="24"/>
-      <c r="G25" s="24"/>
-      <c r="H25" s="26"/>
-      <c r="I25" s="27"/>
-      <c r="J25" s="6"/>
+      <c r="A25" s="25"/>
+      <c r="B25" s="26"/>
+      <c r="C25" s="26"/>
+      <c r="D25" s="6"/>
+      <c r="E25" s="9"/>
+      <c r="F25" s="6"/>
+      <c r="G25" s="6"/>
+      <c r="H25" s="11"/>
+      <c r="I25" s="12"/>
+      <c r="J25" s="2"/>
     </row>
     <row r="26" spans="1:10" ht="20.100000000000001" customHeight="1">
-      <c r="A26" s="11"/>
-      <c r="B26" s="10"/>
-      <c r="C26" s="10"/>
-      <c r="D26" s="24"/>
-      <c r="E26" s="31"/>
-      <c r="F26" s="24"/>
-      <c r="G26" s="24"/>
-      <c r="H26" s="26"/>
-      <c r="I26" s="27"/>
-      <c r="J26" s="6"/>
+      <c r="A26" s="25"/>
+      <c r="B26" s="26"/>
+      <c r="C26" s="26"/>
+      <c r="D26" s="6"/>
+      <c r="E26" s="9"/>
+      <c r="F26" s="6"/>
+      <c r="G26" s="6"/>
+      <c r="H26" s="11"/>
+      <c r="I26" s="12"/>
+      <c r="J26" s="2"/>
     </row>
     <row r="27" spans="1:10" ht="20.100000000000001" customHeight="1">
-      <c r="A27" s="11"/>
-      <c r="B27" s="10"/>
-      <c r="C27" s="10"/>
-      <c r="D27" s="24"/>
-      <c r="E27" s="31"/>
-      <c r="F27" s="24"/>
-      <c r="G27" s="24"/>
-      <c r="H27" s="26"/>
-      <c r="I27" s="27"/>
-      <c r="J27" s="6"/>
+      <c r="A27" s="25"/>
+      <c r="B27" s="26"/>
+      <c r="C27" s="26"/>
+      <c r="D27" s="6"/>
+      <c r="E27" s="9"/>
+      <c r="F27" s="6"/>
+      <c r="G27" s="6"/>
+      <c r="H27" s="11"/>
+      <c r="I27" s="12"/>
+      <c r="J27" s="2"/>
     </row>
     <row r="28" spans="1:10" ht="20.100000000000001" customHeight="1">
-      <c r="A28" s="11"/>
-      <c r="B28" s="10"/>
-      <c r="C28" s="10"/>
-      <c r="D28" s="24"/>
-      <c r="E28" s="31"/>
-      <c r="F28" s="24"/>
-      <c r="G28" s="24"/>
-      <c r="H28" s="26"/>
-      <c r="I28" s="27"/>
-      <c r="J28" s="6"/>
+      <c r="A28" s="25"/>
+      <c r="B28" s="26"/>
+      <c r="C28" s="26"/>
+      <c r="D28" s="6"/>
+      <c r="E28" s="9"/>
+      <c r="F28" s="6"/>
+      <c r="G28" s="6"/>
+      <c r="H28" s="11"/>
+      <c r="I28" s="12"/>
+      <c r="J28" s="2"/>
     </row>
     <row r="29" spans="1:10" ht="20.100000000000001" customHeight="1">
-      <c r="A29" s="11"/>
-      <c r="B29" s="10"/>
-      <c r="C29" s="10"/>
-      <c r="D29" s="24"/>
-      <c r="E29" s="31"/>
-      <c r="F29" s="24"/>
-      <c r="G29" s="24"/>
-      <c r="H29" s="26"/>
-      <c r="I29" s="27"/>
-      <c r="J29" s="6"/>
+      <c r="A29" s="25"/>
+      <c r="B29" s="26"/>
+      <c r="C29" s="26"/>
+      <c r="D29" s="6"/>
+      <c r="E29" s="9"/>
+      <c r="F29" s="6"/>
+      <c r="G29" s="6"/>
+      <c r="H29" s="11"/>
+      <c r="I29" s="12"/>
+      <c r="J29" s="2"/>
     </row>
     <row r="30" spans="1:10" ht="20.100000000000001" customHeight="1">
-      <c r="A30" s="11"/>
-      <c r="B30" s="10"/>
-      <c r="C30" s="10"/>
-      <c r="D30" s="24"/>
-      <c r="E30" s="31"/>
-      <c r="F30" s="24"/>
-      <c r="G30" s="24"/>
-      <c r="H30" s="26"/>
-      <c r="I30" s="27"/>
-      <c r="J30" s="6"/>
+      <c r="A30" s="25"/>
+      <c r="B30" s="26"/>
+      <c r="C30" s="26"/>
+      <c r="D30" s="6"/>
+      <c r="E30" s="9"/>
+      <c r="F30" s="6"/>
+      <c r="G30" s="6"/>
+      <c r="H30" s="11"/>
+      <c r="I30" s="12"/>
+      <c r="J30" s="2"/>
     </row>
     <row r="31" spans="1:10" ht="20.100000000000001" customHeight="1">
-      <c r="A31" s="11"/>
-      <c r="B31" s="10"/>
-      <c r="C31" s="10"/>
-      <c r="D31" s="24"/>
-      <c r="E31" s="31"/>
-      <c r="F31" s="24"/>
-      <c r="G31" s="24"/>
-      <c r="H31" s="26"/>
-      <c r="I31" s="27"/>
-      <c r="J31" s="6"/>
+      <c r="A31" s="25"/>
+      <c r="B31" s="26"/>
+      <c r="C31" s="26"/>
+      <c r="D31" s="6"/>
+      <c r="E31" s="9"/>
+      <c r="F31" s="6"/>
+      <c r="G31" s="6"/>
+      <c r="H31" s="11"/>
+      <c r="I31" s="12"/>
+      <c r="J31" s="2"/>
     </row>
     <row r="32" spans="1:10" ht="20.100000000000001" customHeight="1">
-      <c r="A32" s="11"/>
-      <c r="B32" s="10"/>
-      <c r="C32" s="10"/>
-      <c r="D32" s="24"/>
-      <c r="E32" s="31"/>
-      <c r="F32" s="24"/>
-      <c r="G32" s="24"/>
-      <c r="H32" s="26"/>
-      <c r="I32" s="27"/>
-      <c r="J32" s="6"/>
+      <c r="A32" s="25"/>
+      <c r="B32" s="26"/>
+      <c r="C32" s="26"/>
+      <c r="D32" s="6"/>
+      <c r="E32" s="9"/>
+      <c r="F32" s="6"/>
+      <c r="G32" s="6"/>
+      <c r="H32" s="11"/>
+      <c r="I32" s="12"/>
+      <c r="J32" s="2"/>
     </row>
     <row r="33" spans="1:10" ht="20.100000000000001" customHeight="1">
-      <c r="A33" s="11"/>
-      <c r="B33" s="10"/>
-      <c r="C33" s="10"/>
-      <c r="D33" s="24"/>
-      <c r="E33" s="31"/>
-      <c r="F33" s="24"/>
-      <c r="G33" s="24"/>
-      <c r="H33" s="26"/>
-      <c r="I33" s="27"/>
-      <c r="J33" s="6"/>
+      <c r="A33" s="25"/>
+      <c r="B33" s="26"/>
+      <c r="C33" s="26"/>
+      <c r="D33" s="6"/>
+      <c r="E33" s="9"/>
+      <c r="F33" s="6"/>
+      <c r="G33" s="6"/>
+      <c r="H33" s="11"/>
+      <c r="I33" s="12"/>
+      <c r="J33" s="2"/>
     </row>
     <row r="34" spans="1:10" ht="20.100000000000001" customHeight="1">
-      <c r="A34" s="11"/>
-      <c r="B34" s="10"/>
-      <c r="C34" s="10"/>
-      <c r="D34" s="24"/>
-      <c r="E34" s="31"/>
-      <c r="F34" s="24"/>
-      <c r="G34" s="24"/>
-      <c r="H34" s="26"/>
-      <c r="I34" s="27"/>
-      <c r="J34" s="6"/>
+      <c r="A34" s="25"/>
+      <c r="B34" s="26"/>
+      <c r="C34" s="26"/>
+      <c r="D34" s="6"/>
+      <c r="E34" s="9"/>
+      <c r="F34" s="6"/>
+      <c r="G34" s="6"/>
+      <c r="H34" s="11"/>
+      <c r="I34" s="12"/>
+      <c r="J34" s="2"/>
     </row>
     <row r="35" spans="1:10" ht="20.100000000000001" customHeight="1">
-      <c r="A35" s="11"/>
-      <c r="B35" s="10"/>
-      <c r="C35" s="10"/>
-      <c r="D35" s="24"/>
-      <c r="E35" s="31"/>
-      <c r="F35" s="24"/>
-      <c r="G35" s="24"/>
-      <c r="H35" s="26"/>
-      <c r="I35" s="27"/>
-      <c r="J35" s="6"/>
+      <c r="A35" s="25"/>
+      <c r="B35" s="26"/>
+      <c r="C35" s="26"/>
+      <c r="D35" s="6"/>
+      <c r="E35" s="9"/>
+      <c r="F35" s="6"/>
+      <c r="G35" s="6"/>
+      <c r="H35" s="11"/>
+      <c r="I35" s="12"/>
+      <c r="J35" s="2"/>
     </row>
     <row r="36" spans="1:10" ht="20.100000000000001" customHeight="1">
-      <c r="A36" s="11"/>
-      <c r="B36" s="10"/>
-      <c r="C36" s="10"/>
-      <c r="D36" s="24"/>
-      <c r="E36" s="31"/>
-      <c r="F36" s="24"/>
-      <c r="G36" s="24"/>
-      <c r="H36" s="26"/>
-      <c r="I36" s="27"/>
-      <c r="J36" s="6"/>
+      <c r="A36" s="25"/>
+      <c r="B36" s="26"/>
+      <c r="C36" s="26"/>
+      <c r="D36" s="6"/>
+      <c r="E36" s="9"/>
+      <c r="F36" s="6"/>
+      <c r="G36" s="6"/>
+      <c r="H36" s="11"/>
+      <c r="I36" s="12"/>
+      <c r="J36" s="2"/>
     </row>
     <row r="37" spans="1:10" ht="20.100000000000001" customHeight="1" thickBot="1">
-      <c r="A37" s="12"/>
-      <c r="B37" s="13"/>
-      <c r="C37" s="13"/>
-      <c r="D37" s="24"/>
-      <c r="E37" s="32"/>
-      <c r="F37" s="28"/>
-      <c r="G37" s="28"/>
-      <c r="H37" s="29"/>
-      <c r="I37" s="30"/>
-      <c r="J37" s="6"/>
+      <c r="A37" s="27"/>
+      <c r="B37" s="28"/>
+      <c r="C37" s="28"/>
+      <c r="D37" s="6"/>
+      <c r="E37" s="10"/>
+      <c r="F37" s="8"/>
+      <c r="G37" s="8"/>
+      <c r="H37" s="13"/>
+      <c r="I37" s="14"/>
+      <c r="J37" s="2"/>
     </row>
     <row r="38" spans="1:10" ht="20.100000000000001" customHeight="1">
       <c r="A38" s="1"/>
@@ -1499,6 +1519,61 @@
     </row>
   </sheetData>
   <mergeCells count="71">
+    <mergeCell ref="A4:C4"/>
+    <mergeCell ref="A3:C3"/>
+    <mergeCell ref="A5:C5"/>
+    <mergeCell ref="A6:C6"/>
+    <mergeCell ref="A7:C7"/>
+    <mergeCell ref="A19:C19"/>
+    <mergeCell ref="A8:C8"/>
+    <mergeCell ref="A9:C9"/>
+    <mergeCell ref="A10:C10"/>
+    <mergeCell ref="A11:C11"/>
+    <mergeCell ref="A12:C12"/>
+    <mergeCell ref="A13:C13"/>
+    <mergeCell ref="A34:C34"/>
+    <mergeCell ref="A35:C35"/>
+    <mergeCell ref="A36:C36"/>
+    <mergeCell ref="A37:C37"/>
+    <mergeCell ref="A26:C26"/>
+    <mergeCell ref="A27:C27"/>
+    <mergeCell ref="A28:C28"/>
+    <mergeCell ref="A29:C29"/>
+    <mergeCell ref="A30:C30"/>
+    <mergeCell ref="A31:C31"/>
+    <mergeCell ref="H9:I9"/>
+    <mergeCell ref="H10:I10"/>
+    <mergeCell ref="H11:I11"/>
+    <mergeCell ref="A32:C32"/>
+    <mergeCell ref="A33:C33"/>
+    <mergeCell ref="A20:C20"/>
+    <mergeCell ref="A21:C21"/>
+    <mergeCell ref="A22:C22"/>
+    <mergeCell ref="A23:C23"/>
+    <mergeCell ref="A24:C24"/>
+    <mergeCell ref="A25:C25"/>
+    <mergeCell ref="A14:C14"/>
+    <mergeCell ref="A15:C15"/>
+    <mergeCell ref="A16:C16"/>
+    <mergeCell ref="A17:C17"/>
+    <mergeCell ref="A18:C18"/>
+    <mergeCell ref="H4:I4"/>
+    <mergeCell ref="H5:I5"/>
+    <mergeCell ref="H6:I6"/>
+    <mergeCell ref="H7:I7"/>
+    <mergeCell ref="H8:I8"/>
+    <mergeCell ref="H23:I23"/>
+    <mergeCell ref="H12:I12"/>
+    <mergeCell ref="H13:I13"/>
+    <mergeCell ref="H14:I14"/>
+    <mergeCell ref="H15:I15"/>
+    <mergeCell ref="H16:I16"/>
+    <mergeCell ref="H17:I17"/>
+    <mergeCell ref="H18:I18"/>
+    <mergeCell ref="H19:I19"/>
+    <mergeCell ref="H20:I20"/>
+    <mergeCell ref="H21:I21"/>
+    <mergeCell ref="H22:I22"/>
     <mergeCell ref="H36:I36"/>
     <mergeCell ref="H37:I37"/>
     <mergeCell ref="H3:I3"/>
@@ -1515,61 +1590,6 @@
     <mergeCell ref="H27:I27"/>
     <mergeCell ref="H28:I28"/>
     <mergeCell ref="H29:I29"/>
-    <mergeCell ref="H18:I18"/>
-    <mergeCell ref="H19:I19"/>
-    <mergeCell ref="H20:I20"/>
-    <mergeCell ref="H21:I21"/>
-    <mergeCell ref="H22:I22"/>
-    <mergeCell ref="H23:I23"/>
-    <mergeCell ref="H12:I12"/>
-    <mergeCell ref="H13:I13"/>
-    <mergeCell ref="H14:I14"/>
-    <mergeCell ref="H15:I15"/>
-    <mergeCell ref="H16:I16"/>
-    <mergeCell ref="H17:I17"/>
-    <mergeCell ref="H4:I4"/>
-    <mergeCell ref="H5:I5"/>
-    <mergeCell ref="H6:I6"/>
-    <mergeCell ref="H7:I7"/>
-    <mergeCell ref="H8:I8"/>
-    <mergeCell ref="H9:I9"/>
-    <mergeCell ref="H10:I10"/>
-    <mergeCell ref="H11:I11"/>
-    <mergeCell ref="A32:C32"/>
-    <mergeCell ref="A33:C33"/>
-    <mergeCell ref="A34:C34"/>
-    <mergeCell ref="A35:C35"/>
-    <mergeCell ref="A36:C36"/>
-    <mergeCell ref="A37:C37"/>
-    <mergeCell ref="A26:C26"/>
-    <mergeCell ref="A27:C27"/>
-    <mergeCell ref="A28:C28"/>
-    <mergeCell ref="A29:C29"/>
-    <mergeCell ref="A30:C30"/>
-    <mergeCell ref="A31:C31"/>
-    <mergeCell ref="A20:C20"/>
-    <mergeCell ref="A21:C21"/>
-    <mergeCell ref="A22:C22"/>
-    <mergeCell ref="A23:C23"/>
-    <mergeCell ref="A24:C24"/>
-    <mergeCell ref="A25:C25"/>
-    <mergeCell ref="A14:C14"/>
-    <mergeCell ref="A15:C15"/>
-    <mergeCell ref="A16:C16"/>
-    <mergeCell ref="A17:C17"/>
-    <mergeCell ref="A18:C18"/>
-    <mergeCell ref="A19:C19"/>
-    <mergeCell ref="A8:C8"/>
-    <mergeCell ref="A9:C9"/>
-    <mergeCell ref="A10:C10"/>
-    <mergeCell ref="A11:C11"/>
-    <mergeCell ref="A12:C12"/>
-    <mergeCell ref="A13:C13"/>
-    <mergeCell ref="A4:C4"/>
-    <mergeCell ref="A3:C3"/>
-    <mergeCell ref="A5:C5"/>
-    <mergeCell ref="A6:C6"/>
-    <mergeCell ref="A7:C7"/>
   </mergeCells>
   <pageMargins left="0.25" right="0.25" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" verticalDpi="0" r:id="rId1"/>

</xml_diff>